<commit_message>
pruebas de perfilies y menuV2
</commit_message>
<xml_diff>
--- a/provisional/inserts.xlsx
+++ b/provisional/inserts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="21720" windowHeight="10035" activeTab="5"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="21720" windowHeight="10035" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="inserts iniciales" sheetId="3" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2653" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2542" uniqueCount="245">
   <si>
     <t>NULL</t>
   </si>
@@ -11903,10 +11903,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G185"/>
+  <dimension ref="A1:G148"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11918,8 +11918,8 @@
       <c r="B1" s="1">
         <v>1</v>
       </c>
-      <c r="C1" s="1">
-        <v>1</v>
+      <c r="C1">
+        <v>31</v>
       </c>
       <c r="D1" s="1">
         <v>1</v>
@@ -11941,8 +11941,8 @@
       <c r="B2">
         <v>2</v>
       </c>
-      <c r="C2" s="1">
-        <v>2</v>
+      <c r="C2">
+        <v>32</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
@@ -11964,8 +11964,8 @@
       <c r="B3" s="1">
         <v>3</v>
       </c>
-      <c r="C3" s="1">
-        <v>3</v>
+      <c r="C3">
+        <v>33</v>
       </c>
       <c r="D3" s="1">
         <v>1</v>
@@ -11987,8 +11987,8 @@
       <c r="B4">
         <v>4</v>
       </c>
-      <c r="C4" s="1">
-        <v>4</v>
+      <c r="C4">
+        <v>34</v>
       </c>
       <c r="D4" s="1">
         <v>1</v>
@@ -12010,8 +12010,8 @@
       <c r="B5" s="1">
         <v>5</v>
       </c>
-      <c r="C5" s="1">
-        <v>5</v>
+      <c r="C5">
+        <v>35</v>
       </c>
       <c r="D5" s="1">
         <v>1</v>
@@ -12033,8 +12033,8 @@
       <c r="B6">
         <v>6</v>
       </c>
-      <c r="C6" s="1">
-        <v>6</v>
+      <c r="C6">
+        <v>36</v>
       </c>
       <c r="D6" s="1">
         <v>1</v>
@@ -12056,8 +12056,8 @@
       <c r="B7" s="1">
         <v>7</v>
       </c>
-      <c r="C7" s="1">
-        <v>7</v>
+      <c r="C7">
+        <v>37</v>
       </c>
       <c r="D7" s="1">
         <v>1</v>
@@ -12079,8 +12079,8 @@
       <c r="B8">
         <v>8</v>
       </c>
-      <c r="C8" s="1">
-        <v>8</v>
+      <c r="C8">
+        <v>38</v>
       </c>
       <c r="D8" s="1">
         <v>1</v>
@@ -12102,8 +12102,8 @@
       <c r="B9" s="1">
         <v>9</v>
       </c>
-      <c r="C9" s="1">
-        <v>9</v>
+      <c r="C9">
+        <v>39</v>
       </c>
       <c r="D9" s="1">
         <v>1</v>
@@ -12125,8 +12125,8 @@
       <c r="B10">
         <v>10</v>
       </c>
-      <c r="C10" s="1">
-        <v>10</v>
+      <c r="C10">
+        <v>40</v>
       </c>
       <c r="D10" s="1">
         <v>1</v>
@@ -12148,8 +12148,8 @@
       <c r="B11" s="1">
         <v>11</v>
       </c>
-      <c r="C11" s="1">
-        <v>11</v>
+      <c r="C11">
+        <v>41</v>
       </c>
       <c r="D11" s="1">
         <v>1</v>
@@ -12171,8 +12171,8 @@
       <c r="B12">
         <v>12</v>
       </c>
-      <c r="C12" s="1">
-        <v>12</v>
+      <c r="C12">
+        <v>42</v>
       </c>
       <c r="D12" s="1">
         <v>1</v>
@@ -12194,8 +12194,8 @@
       <c r="B13" s="1">
         <v>13</v>
       </c>
-      <c r="C13" s="1">
-        <v>13</v>
+      <c r="C13">
+        <v>43</v>
       </c>
       <c r="D13" s="1">
         <v>1</v>
@@ -12217,8 +12217,8 @@
       <c r="B14">
         <v>14</v>
       </c>
-      <c r="C14" s="1">
-        <v>14</v>
+      <c r="C14">
+        <v>44</v>
       </c>
       <c r="D14" s="1">
         <v>1</v>
@@ -12240,8 +12240,8 @@
       <c r="B15" s="1">
         <v>15</v>
       </c>
-      <c r="C15" s="1">
-        <v>15</v>
+      <c r="C15">
+        <v>45</v>
       </c>
       <c r="D15" s="1">
         <v>1</v>
@@ -12264,7 +12264,7 @@
         <v>16</v>
       </c>
       <c r="C16">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D16" s="1">
         <v>2</v>
@@ -12287,7 +12287,7 @@
         <v>17</v>
       </c>
       <c r="C17">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="D17" s="1">
         <v>2</v>
@@ -12310,7 +12310,7 @@
         <v>18</v>
       </c>
       <c r="C18">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="D18" s="1">
         <v>2</v>
@@ -12333,7 +12333,7 @@
         <v>19</v>
       </c>
       <c r="C19">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="D19" s="1">
         <v>2</v>
@@ -12356,7 +12356,7 @@
         <v>20</v>
       </c>
       <c r="C20">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="D20" s="1">
         <v>2</v>
@@ -12379,7 +12379,7 @@
         <v>21</v>
       </c>
       <c r="C21">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="D21" s="1">
         <v>2</v>
@@ -12402,7 +12402,7 @@
         <v>22</v>
       </c>
       <c r="C22">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="D22" s="1">
         <v>2</v>
@@ -12425,7 +12425,7 @@
         <v>23</v>
       </c>
       <c r="C23">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="D23" s="1">
         <v>2</v>
@@ -12448,7 +12448,7 @@
         <v>24</v>
       </c>
       <c r="C24">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="D24" s="1">
         <v>2</v>
@@ -12471,7 +12471,7 @@
         <v>25</v>
       </c>
       <c r="C25">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="D25" s="1">
         <v>2</v>
@@ -12494,7 +12494,7 @@
         <v>26</v>
       </c>
       <c r="C26">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="D26" s="1">
         <v>2</v>
@@ -12517,7 +12517,7 @@
         <v>27</v>
       </c>
       <c r="C27">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="D27" s="1">
         <v>2</v>
@@ -12540,7 +12540,7 @@
         <v>28</v>
       </c>
       <c r="C28">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="D28" s="1">
         <v>2</v>
@@ -12563,7 +12563,7 @@
         <v>29</v>
       </c>
       <c r="C29">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="D29">
         <v>3</v>
@@ -12586,7 +12586,7 @@
         <v>30</v>
       </c>
       <c r="C30">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="D30">
         <v>3</v>
@@ -12609,7 +12609,7 @@
         <v>31</v>
       </c>
       <c r="C31">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="D31">
         <v>3</v>
@@ -12632,7 +12632,7 @@
         <v>32</v>
       </c>
       <c r="C32">
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="D32">
         <v>3</v>
@@ -12655,7 +12655,7 @@
         <v>33</v>
       </c>
       <c r="C33">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="D33">
         <v>3</v>
@@ -12678,7 +12678,7 @@
         <v>34</v>
       </c>
       <c r="C34">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="D34">
         <v>3</v>
@@ -12701,7 +12701,7 @@
         <v>35</v>
       </c>
       <c r="C35">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="D35">
         <v>3</v>
@@ -12724,7 +12724,7 @@
         <v>36</v>
       </c>
       <c r="C36">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="D36">
         <v>3</v>
@@ -12747,7 +12747,7 @@
         <v>37</v>
       </c>
       <c r="C37">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="D37">
         <v>3</v>
@@ -12770,7 +12770,7 @@
         <v>38</v>
       </c>
       <c r="C38">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="D38">
         <v>3</v>
@@ -12793,7 +12793,7 @@
         <v>39</v>
       </c>
       <c r="C39">
-        <v>39</v>
+        <v>69</v>
       </c>
       <c r="D39">
         <v>3</v>
@@ -12815,8 +12815,8 @@
       <c r="B40" s="1">
         <v>40</v>
       </c>
-      <c r="C40" s="1">
-        <v>40</v>
+      <c r="C40">
+        <v>70</v>
       </c>
       <c r="D40">
         <v>3</v>
@@ -12839,7 +12839,7 @@
         <v>41</v>
       </c>
       <c r="C41">
-        <v>41</v>
+        <v>71</v>
       </c>
       <c r="D41">
         <v>4</v>
@@ -12862,7 +12862,7 @@
         <v>42</v>
       </c>
       <c r="C42">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="D42">
         <v>4</v>
@@ -12885,7 +12885,7 @@
         <v>43</v>
       </c>
       <c r="C43">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="D43">
         <v>4</v>
@@ -12908,7 +12908,7 @@
         <v>44</v>
       </c>
       <c r="C44">
-        <v>44</v>
+        <v>74</v>
       </c>
       <c r="D44">
         <v>4</v>
@@ -12931,7 +12931,7 @@
         <v>45</v>
       </c>
       <c r="C45">
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="D45">
         <v>4</v>
@@ -12954,7 +12954,7 @@
         <v>46</v>
       </c>
       <c r="C46">
-        <v>46</v>
+        <v>76</v>
       </c>
       <c r="D46">
         <v>4</v>
@@ -12977,7 +12977,7 @@
         <v>47</v>
       </c>
       <c r="C47">
-        <v>47</v>
+        <v>77</v>
       </c>
       <c r="D47">
         <v>4</v>
@@ -13000,7 +13000,7 @@
         <v>48</v>
       </c>
       <c r="C48">
-        <v>48</v>
+        <v>78</v>
       </c>
       <c r="D48">
         <v>4</v>
@@ -13023,7 +13023,7 @@
         <v>49</v>
       </c>
       <c r="C49">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="D49">
         <v>4</v>
@@ -13046,7 +13046,7 @@
         <v>50</v>
       </c>
       <c r="C50">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="D50">
         <v>4</v>
@@ -13069,7 +13069,7 @@
         <v>51</v>
       </c>
       <c r="C51">
-        <v>51</v>
+        <v>81</v>
       </c>
       <c r="D51">
         <v>4</v>
@@ -13092,7 +13092,7 @@
         <v>52</v>
       </c>
       <c r="C52">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="D52">
         <v>4</v>
@@ -13115,7 +13115,7 @@
         <v>53</v>
       </c>
       <c r="C53">
-        <v>53</v>
+        <v>83</v>
       </c>
       <c r="D53">
         <v>4</v>
@@ -13138,7 +13138,7 @@
         <v>54</v>
       </c>
       <c r="C54">
-        <v>54</v>
+        <v>84</v>
       </c>
       <c r="D54">
         <v>4</v>
@@ -13161,7 +13161,7 @@
         <v>55</v>
       </c>
       <c r="C55">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="D55">
         <v>4</v>
@@ -13184,7 +13184,7 @@
         <v>56</v>
       </c>
       <c r="C56">
-        <v>56</v>
+        <v>86</v>
       </c>
       <c r="D56">
         <v>4</v>
@@ -13207,7 +13207,7 @@
         <v>57</v>
       </c>
       <c r="C57">
-        <v>57</v>
+        <v>87</v>
       </c>
       <c r="D57">
         <v>5</v>
@@ -13230,7 +13230,7 @@
         <v>58</v>
       </c>
       <c r="C58">
-        <v>58</v>
+        <v>88</v>
       </c>
       <c r="D58">
         <v>5</v>
@@ -13253,7 +13253,7 @@
         <v>59</v>
       </c>
       <c r="C59">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="D59">
         <v>5</v>
@@ -13276,7 +13276,7 @@
         <v>60</v>
       </c>
       <c r="C60">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="D60">
         <v>5</v>
@@ -13299,7 +13299,7 @@
         <v>61</v>
       </c>
       <c r="C61">
-        <v>61</v>
+        <v>91</v>
       </c>
       <c r="D61">
         <v>5</v>
@@ -13322,7 +13322,7 @@
         <v>62</v>
       </c>
       <c r="C62">
-        <v>62</v>
+        <v>92</v>
       </c>
       <c r="D62">
         <v>5</v>
@@ -13345,7 +13345,7 @@
         <v>63</v>
       </c>
       <c r="C63">
-        <v>63</v>
+        <v>93</v>
       </c>
       <c r="D63">
         <v>5</v>
@@ -13368,7 +13368,7 @@
         <v>64</v>
       </c>
       <c r="C64">
-        <v>64</v>
+        <v>94</v>
       </c>
       <c r="D64">
         <v>5</v>
@@ -13391,7 +13391,7 @@
         <v>65</v>
       </c>
       <c r="C65">
-        <v>65</v>
+        <v>95</v>
       </c>
       <c r="D65">
         <v>5</v>
@@ -13414,7 +13414,7 @@
         <v>66</v>
       </c>
       <c r="C66">
-        <v>66</v>
+        <v>96</v>
       </c>
       <c r="D66">
         <v>5</v>
@@ -13437,7 +13437,7 @@
         <v>67</v>
       </c>
       <c r="C67">
-        <v>67</v>
+        <v>97</v>
       </c>
       <c r="D67">
         <v>5</v>
@@ -13460,7 +13460,7 @@
         <v>68</v>
       </c>
       <c r="C68">
-        <v>68</v>
+        <v>98</v>
       </c>
       <c r="D68">
         <v>5</v>
@@ -13483,7 +13483,7 @@
         <v>69</v>
       </c>
       <c r="C69">
-        <v>69</v>
+        <v>99</v>
       </c>
       <c r="D69">
         <v>5</v>
@@ -13506,7 +13506,7 @@
         <v>70</v>
       </c>
       <c r="C70">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="D70">
         <v>6</v>
@@ -13529,7 +13529,7 @@
         <v>71</v>
       </c>
       <c r="C71">
-        <v>71</v>
+        <v>101</v>
       </c>
       <c r="D71">
         <v>6</v>
@@ -13552,7 +13552,7 @@
         <v>72</v>
       </c>
       <c r="C72">
-        <v>72</v>
+        <v>102</v>
       </c>
       <c r="D72">
         <v>6</v>
@@ -13575,7 +13575,7 @@
         <v>73</v>
       </c>
       <c r="C73">
-        <v>73</v>
+        <v>103</v>
       </c>
       <c r="D73">
         <v>6</v>
@@ -13598,7 +13598,7 @@
         <v>74</v>
       </c>
       <c r="C74">
-        <v>74</v>
+        <v>104</v>
       </c>
       <c r="D74">
         <v>6</v>
@@ -13621,7 +13621,7 @@
         <v>75</v>
       </c>
       <c r="C75">
-        <v>75</v>
+        <v>105</v>
       </c>
       <c r="D75">
         <v>6</v>
@@ -13644,7 +13644,7 @@
         <v>76</v>
       </c>
       <c r="C76">
-        <v>76</v>
+        <v>106</v>
       </c>
       <c r="D76">
         <v>6</v>
@@ -13667,7 +13667,7 @@
         <v>77</v>
       </c>
       <c r="C77">
-        <v>77</v>
+        <v>107</v>
       </c>
       <c r="D77">
         <v>6</v>
@@ -13690,7 +13690,7 @@
         <v>78</v>
       </c>
       <c r="C78">
-        <v>78</v>
+        <v>108</v>
       </c>
       <c r="D78">
         <v>6</v>
@@ -13713,7 +13713,7 @@
         <v>79</v>
       </c>
       <c r="C79">
-        <v>79</v>
+        <v>109</v>
       </c>
       <c r="D79">
         <v>6</v>
@@ -13736,7 +13736,7 @@
         <v>80</v>
       </c>
       <c r="C80">
-        <v>80</v>
+        <v>110</v>
       </c>
       <c r="D80">
         <v>6</v>
@@ -13759,7 +13759,7 @@
         <v>81</v>
       </c>
       <c r="C81">
-        <v>81</v>
+        <v>111</v>
       </c>
       <c r="D81">
         <v>6</v>
@@ -13782,7 +13782,7 @@
         <v>82</v>
       </c>
       <c r="C82">
-        <v>82</v>
+        <v>112</v>
       </c>
       <c r="D82">
         <v>6</v>
@@ -13805,7 +13805,7 @@
         <v>83</v>
       </c>
       <c r="C83">
-        <v>83</v>
+        <v>113</v>
       </c>
       <c r="D83">
         <v>6</v>
@@ -13828,7 +13828,7 @@
         <v>84</v>
       </c>
       <c r="C84">
-        <v>84</v>
+        <v>114</v>
       </c>
       <c r="D84">
         <v>6</v>
@@ -13851,7 +13851,7 @@
         <v>85</v>
       </c>
       <c r="C85">
-        <v>85</v>
+        <v>115</v>
       </c>
       <c r="D85">
         <v>6</v>
@@ -13874,7 +13874,7 @@
         <v>86</v>
       </c>
       <c r="C86">
-        <v>86</v>
+        <v>116</v>
       </c>
       <c r="D86">
         <v>6</v>
@@ -13897,7 +13897,7 @@
         <v>87</v>
       </c>
       <c r="C87">
-        <v>87</v>
+        <v>117</v>
       </c>
       <c r="D87">
         <v>6</v>
@@ -13920,7 +13920,7 @@
         <v>88</v>
       </c>
       <c r="C88">
-        <v>88</v>
+        <v>118</v>
       </c>
       <c r="D88">
         <v>7</v>
@@ -13943,7 +13943,7 @@
         <v>89</v>
       </c>
       <c r="C89">
-        <v>89</v>
+        <v>119</v>
       </c>
       <c r="D89">
         <v>7</v>
@@ -13966,7 +13966,7 @@
         <v>90</v>
       </c>
       <c r="C90">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="D90">
         <v>7</v>
@@ -13989,7 +13989,7 @@
         <v>91</v>
       </c>
       <c r="C91">
-        <v>91</v>
+        <v>121</v>
       </c>
       <c r="D91">
         <v>7</v>
@@ -14012,7 +14012,7 @@
         <v>92</v>
       </c>
       <c r="C92">
-        <v>92</v>
+        <v>122</v>
       </c>
       <c r="D92">
         <v>7</v>
@@ -14035,7 +14035,7 @@
         <v>93</v>
       </c>
       <c r="C93">
-        <v>93</v>
+        <v>123</v>
       </c>
       <c r="D93">
         <v>7</v>
@@ -14058,7 +14058,7 @@
         <v>94</v>
       </c>
       <c r="C94">
-        <v>94</v>
+        <v>124</v>
       </c>
       <c r="D94">
         <v>7</v>
@@ -14081,7 +14081,7 @@
         <v>95</v>
       </c>
       <c r="C95">
-        <v>95</v>
+        <v>125</v>
       </c>
       <c r="D95">
         <v>7</v>
@@ -14104,7 +14104,7 @@
         <v>96</v>
       </c>
       <c r="C96">
-        <v>96</v>
+        <v>126</v>
       </c>
       <c r="D96">
         <v>7</v>
@@ -14127,7 +14127,7 @@
         <v>97</v>
       </c>
       <c r="C97">
-        <v>97</v>
+        <v>127</v>
       </c>
       <c r="D97">
         <v>7</v>
@@ -14150,7 +14150,7 @@
         <v>98</v>
       </c>
       <c r="C98">
-        <v>98</v>
+        <v>128</v>
       </c>
       <c r="D98">
         <v>8</v>
@@ -14173,7 +14173,7 @@
         <v>99</v>
       </c>
       <c r="C99">
-        <v>99</v>
+        <v>129</v>
       </c>
       <c r="D99">
         <v>8</v>
@@ -14196,7 +14196,7 @@
         <v>100</v>
       </c>
       <c r="C100">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="D100">
         <v>8</v>
@@ -14219,7 +14219,7 @@
         <v>101</v>
       </c>
       <c r="C101">
-        <v>101</v>
+        <v>131</v>
       </c>
       <c r="D101">
         <v>8</v>
@@ -14242,7 +14242,7 @@
         <v>102</v>
       </c>
       <c r="C102">
-        <v>102</v>
+        <v>132</v>
       </c>
       <c r="D102">
         <v>8</v>
@@ -14265,7 +14265,7 @@
         <v>103</v>
       </c>
       <c r="C103">
-        <v>103</v>
+        <v>133</v>
       </c>
       <c r="D103">
         <v>8</v>
@@ -14288,7 +14288,7 @@
         <v>104</v>
       </c>
       <c r="C104">
-        <v>104</v>
+        <v>134</v>
       </c>
       <c r="D104">
         <v>8</v>
@@ -14311,7 +14311,7 @@
         <v>105</v>
       </c>
       <c r="C105">
-        <v>105</v>
+        <v>135</v>
       </c>
       <c r="D105">
         <v>8</v>
@@ -14334,7 +14334,7 @@
         <v>106</v>
       </c>
       <c r="C106">
-        <v>106</v>
+        <v>136</v>
       </c>
       <c r="D106">
         <v>8</v>
@@ -14357,7 +14357,7 @@
         <v>107</v>
       </c>
       <c r="C107">
-        <v>107</v>
+        <v>137</v>
       </c>
       <c r="D107">
         <v>8</v>
@@ -14380,7 +14380,7 @@
         <v>108</v>
       </c>
       <c r="C108">
-        <v>108</v>
+        <v>138</v>
       </c>
       <c r="D108">
         <v>8</v>
@@ -14403,7 +14403,7 @@
         <v>109</v>
       </c>
       <c r="C109">
-        <v>109</v>
+        <v>139</v>
       </c>
       <c r="D109">
         <v>8</v>
@@ -14426,7 +14426,7 @@
         <v>110</v>
       </c>
       <c r="C110">
-        <v>110</v>
+        <v>140</v>
       </c>
       <c r="D110">
         <v>8</v>
@@ -14449,7 +14449,7 @@
         <v>111</v>
       </c>
       <c r="C111">
-        <v>111</v>
+        <v>141</v>
       </c>
       <c r="D111">
         <v>8</v>
@@ -14472,7 +14472,7 @@
         <v>112</v>
       </c>
       <c r="C112">
-        <v>112</v>
+        <v>142</v>
       </c>
       <c r="D112">
         <v>8</v>
@@ -14495,7 +14495,7 @@
         <v>113</v>
       </c>
       <c r="C113">
-        <v>113</v>
+        <v>143</v>
       </c>
       <c r="D113">
         <v>8</v>
@@ -14518,7 +14518,7 @@
         <v>114</v>
       </c>
       <c r="C114">
-        <v>114</v>
+        <v>144</v>
       </c>
       <c r="D114">
         <v>8</v>
@@ -14541,7 +14541,7 @@
         <v>115</v>
       </c>
       <c r="C115">
-        <v>115</v>
+        <v>145</v>
       </c>
       <c r="D115">
         <v>8</v>
@@ -14564,7 +14564,7 @@
         <v>116</v>
       </c>
       <c r="C116">
-        <v>116</v>
+        <v>146</v>
       </c>
       <c r="D116">
         <v>8</v>
@@ -14587,7 +14587,7 @@
         <v>117</v>
       </c>
       <c r="C117">
-        <v>117</v>
+        <v>147</v>
       </c>
       <c r="D117">
         <v>8</v>
@@ -14610,7 +14610,7 @@
         <v>118</v>
       </c>
       <c r="C118">
-        <v>118</v>
+        <v>148</v>
       </c>
       <c r="D118">
         <v>8</v>
@@ -14627,623 +14627,623 @@
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
-        <v>1</v>
-      </c>
-      <c r="B119">
-        <v>119</v>
+        <v>2</v>
+      </c>
+      <c r="B119" s="1">
+        <v>1</v>
       </c>
       <c r="C119">
-        <v>119</v>
-      </c>
-      <c r="D119">
-        <v>8</v>
+        <v>103</v>
+      </c>
+      <c r="D119" s="1">
+        <v>2</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="G119" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
-        <v>1</v>
-      </c>
-      <c r="B120">
-        <v>120</v>
+        <v>2</v>
+      </c>
+      <c r="B120" s="1">
+        <v>2</v>
       </c>
       <c r="C120">
-        <v>120</v>
-      </c>
-      <c r="D120">
-        <v>9</v>
+        <v>104</v>
+      </c>
+      <c r="D120" s="1">
+        <v>2</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="G120" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
-        <v>1</v>
-      </c>
-      <c r="B121">
-        <v>121</v>
+        <v>2</v>
+      </c>
+      <c r="B121" s="1">
+        <v>3</v>
       </c>
       <c r="C121">
-        <v>121</v>
-      </c>
-      <c r="D121">
-        <v>9</v>
+        <v>105</v>
+      </c>
+      <c r="D121" s="1">
+        <v>2</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="G121" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
-        <v>1</v>
-      </c>
-      <c r="B122">
-        <v>122</v>
+        <v>2</v>
+      </c>
+      <c r="B122" s="1">
+        <v>4</v>
       </c>
       <c r="C122">
-        <v>122</v>
-      </c>
-      <c r="D122">
-        <v>9</v>
+        <v>110</v>
+      </c>
+      <c r="D122" s="1">
+        <v>2</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="G122" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
-        <v>1</v>
-      </c>
-      <c r="B123">
-        <v>123</v>
+        <v>2</v>
+      </c>
+      <c r="B123" s="1">
+        <v>5</v>
       </c>
       <c r="C123">
-        <v>123</v>
-      </c>
-      <c r="D123">
-        <v>9</v>
+        <v>111</v>
+      </c>
+      <c r="D123" s="1">
+        <v>2</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="G123" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
-        <v>1</v>
-      </c>
-      <c r="B124">
-        <v>124</v>
+        <v>2</v>
+      </c>
+      <c r="B124" s="1">
+        <v>6</v>
       </c>
       <c r="C124">
-        <v>124</v>
-      </c>
-      <c r="D124">
-        <v>9</v>
+        <v>112</v>
+      </c>
+      <c r="D124" s="1">
+        <v>2</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="G124" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
-        <v>1</v>
-      </c>
-      <c r="B125">
-        <v>125</v>
+        <v>2</v>
+      </c>
+      <c r="B125" s="1">
+        <v>7</v>
       </c>
       <c r="C125">
-        <v>125</v>
-      </c>
-      <c r="D125">
-        <v>9</v>
+        <v>113</v>
+      </c>
+      <c r="D125" s="1">
+        <v>2</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="G125" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
-        <v>1</v>
-      </c>
-      <c r="B126">
-        <v>126</v>
+        <v>2</v>
+      </c>
+      <c r="B126" s="1">
+        <v>8</v>
       </c>
       <c r="C126">
-        <v>126</v>
-      </c>
-      <c r="D126">
-        <v>9</v>
+        <v>114</v>
+      </c>
+      <c r="D126" s="1">
+        <v>2</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="G126" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
-        <v>1</v>
-      </c>
-      <c r="B127">
-        <v>127</v>
+        <v>2</v>
+      </c>
+      <c r="B127" s="1">
+        <v>9</v>
       </c>
       <c r="C127">
-        <v>127</v>
-      </c>
-      <c r="D127">
-        <v>9</v>
+        <v>115</v>
+      </c>
+      <c r="D127" s="1">
+        <v>2</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="G127" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
-        <v>1</v>
-      </c>
-      <c r="B128">
-        <v>128</v>
+        <v>2</v>
+      </c>
+      <c r="B128" s="1">
+        <v>10</v>
       </c>
       <c r="C128">
-        <v>128</v>
-      </c>
-      <c r="D128">
-        <v>9</v>
+        <v>116</v>
+      </c>
+      <c r="D128" s="1">
+        <v>2</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="G128" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
-        <v>1</v>
-      </c>
-      <c r="B129">
-        <v>129</v>
+        <v>2</v>
+      </c>
+      <c r="B129" s="1">
+        <v>11</v>
       </c>
       <c r="C129">
         <v>129</v>
       </c>
-      <c r="D129">
-        <v>9</v>
+      <c r="D129" s="1">
+        <v>2</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="F129" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="G129" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
-        <v>1</v>
-      </c>
-      <c r="B130">
-        <v>130</v>
+        <v>2</v>
+      </c>
+      <c r="B130" s="1">
+        <v>12</v>
       </c>
       <c r="C130">
         <v>130</v>
       </c>
-      <c r="D130">
-        <v>9</v>
+      <c r="D130" s="1">
+        <v>2</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="G130" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
-        <v>1</v>
-      </c>
-      <c r="B131">
-        <v>131</v>
+        <v>2</v>
+      </c>
+      <c r="B131" s="1">
+        <v>13</v>
       </c>
       <c r="C131">
         <v>131</v>
       </c>
-      <c r="D131">
-        <v>9</v>
+      <c r="D131" s="1">
+        <v>3</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="G131" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
-        <v>1</v>
-      </c>
-      <c r="B132">
-        <v>132</v>
+        <v>2</v>
+      </c>
+      <c r="B132" s="1">
+        <v>14</v>
       </c>
       <c r="C132">
-        <v>132</v>
-      </c>
-      <c r="D132">
-        <v>9</v>
+        <v>135</v>
+      </c>
+      <c r="D132" s="1">
+        <v>3</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="G132" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
-        <v>1</v>
-      </c>
-      <c r="B133">
-        <v>133</v>
+        <v>2</v>
+      </c>
+      <c r="B133" s="1">
+        <v>15</v>
       </c>
       <c r="C133">
-        <v>133</v>
-      </c>
-      <c r="D133">
-        <v>9</v>
+        <v>136</v>
+      </c>
+      <c r="D133" s="1">
+        <v>3</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="F133" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="G133" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
-        <v>1</v>
-      </c>
-      <c r="B134">
-        <v>134</v>
+        <v>2</v>
+      </c>
+      <c r="B134" s="1">
+        <v>16</v>
       </c>
       <c r="C134">
-        <v>134</v>
-      </c>
-      <c r="D134">
-        <v>9</v>
+        <v>137</v>
+      </c>
+      <c r="D134" s="1">
+        <v>3</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="F134" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="G134" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
-        <v>1</v>
-      </c>
-      <c r="B135">
-        <v>135</v>
+        <v>2</v>
+      </c>
+      <c r="B135" s="1">
+        <v>17</v>
       </c>
       <c r="C135">
-        <v>135</v>
-      </c>
-      <c r="D135">
-        <v>10</v>
+        <v>138</v>
+      </c>
+      <c r="D135" s="1">
+        <v>3</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="F135" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="G135" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
-        <v>1</v>
-      </c>
-      <c r="B136">
-        <v>136</v>
+        <v>2</v>
+      </c>
+      <c r="B136" s="1">
+        <v>18</v>
       </c>
       <c r="C136">
-        <v>136</v>
-      </c>
-      <c r="D136">
-        <v>10</v>
+        <v>139</v>
+      </c>
+      <c r="D136" s="1">
+        <v>3</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="F136" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="G136" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
-        <v>1</v>
-      </c>
-      <c r="B137">
-        <v>137</v>
+        <v>2</v>
+      </c>
+      <c r="B137" s="1">
+        <v>19</v>
       </c>
       <c r="C137">
-        <v>137</v>
-      </c>
-      <c r="D137">
-        <v>10</v>
+        <v>140</v>
+      </c>
+      <c r="D137" s="1">
+        <v>3</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="F137" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="G137" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
-        <v>1</v>
-      </c>
-      <c r="B138">
-        <v>138</v>
+        <v>2</v>
+      </c>
+      <c r="B138" s="1">
+        <v>20</v>
       </c>
       <c r="C138">
-        <v>138</v>
-      </c>
-      <c r="D138">
-        <v>10</v>
+        <v>46</v>
+      </c>
+      <c r="D138" s="1">
+        <v>3</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="F138" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="G138" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
-        <v>1</v>
-      </c>
-      <c r="B139">
-        <v>139</v>
+        <v>2</v>
+      </c>
+      <c r="B139" s="1">
+        <v>21</v>
       </c>
       <c r="C139">
-        <v>139</v>
-      </c>
-      <c r="D139">
-        <v>10</v>
+        <v>47</v>
+      </c>
+      <c r="D139" s="1">
+        <v>3</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="F139" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="G139" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
-        <v>1</v>
-      </c>
-      <c r="B140">
-        <v>140</v>
+        <v>2</v>
+      </c>
+      <c r="B140" s="1">
+        <v>22</v>
       </c>
       <c r="C140">
-        <v>140</v>
-      </c>
-      <c r="D140">
-        <v>10</v>
+        <v>48</v>
+      </c>
+      <c r="D140" s="1">
+        <v>3</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="F140" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="G140" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
-        <v>1</v>
-      </c>
-      <c r="B141">
-        <v>141</v>
+        <v>2</v>
+      </c>
+      <c r="B141" s="1">
+        <v>23</v>
       </c>
       <c r="C141">
-        <v>141</v>
-      </c>
-      <c r="D141">
-        <v>10</v>
+        <v>49</v>
+      </c>
+      <c r="D141" s="1">
+        <v>3</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="G141" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
-        <v>1</v>
-      </c>
-      <c r="B142">
-        <v>142</v>
+        <v>2</v>
+      </c>
+      <c r="B142" s="1">
+        <v>24</v>
       </c>
       <c r="C142">
-        <v>142</v>
-      </c>
-      <c r="D142">
-        <v>10</v>
+        <v>50</v>
+      </c>
+      <c r="D142" s="1">
+        <v>3</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="F142" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="G142" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
-        <v>1</v>
-      </c>
-      <c r="B143">
-        <v>143</v>
+        <v>2</v>
+      </c>
+      <c r="B143" s="1">
+        <v>25</v>
       </c>
       <c r="C143">
-        <v>143</v>
-      </c>
-      <c r="D143">
-        <v>10</v>
+        <v>51</v>
+      </c>
+      <c r="D143" s="1">
+        <v>6</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="F143" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="G143" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
-        <v>1</v>
-      </c>
-      <c r="B144">
-        <v>144</v>
+        <v>2</v>
+      </c>
+      <c r="B144" s="1">
+        <v>26</v>
       </c>
       <c r="C144">
-        <v>144</v>
-      </c>
-      <c r="D144">
-        <v>10</v>
+        <v>52</v>
+      </c>
+      <c r="D144" s="1">
+        <v>6</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="F144" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="G144" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
-        <v>1</v>
-      </c>
-      <c r="B145">
-        <v>145</v>
+        <v>2</v>
+      </c>
+      <c r="B145" s="1">
+        <v>27</v>
       </c>
       <c r="C145">
-        <v>145</v>
-      </c>
-      <c r="D145">
-        <v>10</v>
+        <v>53</v>
+      </c>
+      <c r="D145" s="1">
+        <v>6</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="F145" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="G145" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.25">
@@ -15251,13 +15251,13 @@
         <v>2</v>
       </c>
       <c r="B146" s="1">
-        <v>1</v>
-      </c>
-      <c r="C146" s="1">
-        <v>16</v>
+        <v>28</v>
+      </c>
+      <c r="C146">
+        <v>54</v>
       </c>
       <c r="D146" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E146" s="1" t="s">
         <v>199</v>
@@ -15274,13 +15274,13 @@
         <v>2</v>
       </c>
       <c r="B147" s="1">
-        <v>2</v>
-      </c>
-      <c r="C147" s="1">
-        <v>17</v>
+        <v>29</v>
+      </c>
+      <c r="C147">
+        <v>55</v>
       </c>
       <c r="D147" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E147" s="1" t="s">
         <v>199</v>
@@ -15294,16 +15294,16 @@
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B148" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C148" s="1">
-        <v>18</v>
+        <v>145</v>
       </c>
       <c r="D148" s="1">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E148" s="1" t="s">
         <v>199</v>
@@ -15312,857 +15312,6 @@
         <v>199</v>
       </c>
       <c r="G148" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A149" s="1">
-        <v>2</v>
-      </c>
-      <c r="B149" s="1">
-        <v>4</v>
-      </c>
-      <c r="C149" s="1">
-        <v>19</v>
-      </c>
-      <c r="D149" s="1">
-        <v>2</v>
-      </c>
-      <c r="E149" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="F149" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="G149" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A150" s="1">
-        <v>2</v>
-      </c>
-      <c r="B150" s="1">
-        <v>5</v>
-      </c>
-      <c r="C150" s="1">
-        <v>20</v>
-      </c>
-      <c r="D150" s="1">
-        <v>2</v>
-      </c>
-      <c r="E150" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="F150" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="G150" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A151" s="1">
-        <v>2</v>
-      </c>
-      <c r="B151" s="1">
-        <v>6</v>
-      </c>
-      <c r="C151" s="1">
-        <v>21</v>
-      </c>
-      <c r="D151" s="1">
-        <v>2</v>
-      </c>
-      <c r="E151" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="F151" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="G151" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A152" s="1">
-        <v>2</v>
-      </c>
-      <c r="B152" s="1">
-        <v>7</v>
-      </c>
-      <c r="C152" s="1">
-        <v>22</v>
-      </c>
-      <c r="D152" s="1">
-        <v>2</v>
-      </c>
-      <c r="E152" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="F152" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="G152" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A153" s="1">
-        <v>2</v>
-      </c>
-      <c r="B153" s="1">
-        <v>8</v>
-      </c>
-      <c r="C153" s="1">
-        <v>23</v>
-      </c>
-      <c r="D153" s="1">
-        <v>2</v>
-      </c>
-      <c r="E153" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="F153" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="G153" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A154" s="1">
-        <v>2</v>
-      </c>
-      <c r="B154" s="1">
-        <v>9</v>
-      </c>
-      <c r="C154" s="1">
-        <v>24</v>
-      </c>
-      <c r="D154" s="1">
-        <v>2</v>
-      </c>
-      <c r="E154" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="F154" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="G154" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A155" s="1">
-        <v>2</v>
-      </c>
-      <c r="B155" s="1">
-        <v>10</v>
-      </c>
-      <c r="C155" s="1">
-        <v>25</v>
-      </c>
-      <c r="D155" s="1">
-        <v>2</v>
-      </c>
-      <c r="E155" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="F155" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="G155" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A156" s="1">
-        <v>2</v>
-      </c>
-      <c r="B156" s="1">
-        <v>11</v>
-      </c>
-      <c r="C156" s="1">
-        <v>26</v>
-      </c>
-      <c r="D156" s="1">
-        <v>2</v>
-      </c>
-      <c r="E156" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="F156" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="G156" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A157" s="1">
-        <v>2</v>
-      </c>
-      <c r="B157" s="1">
-        <v>12</v>
-      </c>
-      <c r="C157" s="1">
-        <v>27</v>
-      </c>
-      <c r="D157" s="1">
-        <v>2</v>
-      </c>
-      <c r="E157" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="F157" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="G157" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A158" s="1">
-        <v>2</v>
-      </c>
-      <c r="B158" s="1">
-        <v>13</v>
-      </c>
-      <c r="C158" s="1">
-        <v>28</v>
-      </c>
-      <c r="D158" s="1">
-        <v>3</v>
-      </c>
-      <c r="E158" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="F158" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="G158" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A159" s="1">
-        <v>2</v>
-      </c>
-      <c r="B159" s="1">
-        <v>14</v>
-      </c>
-      <c r="C159" s="1">
-        <v>29</v>
-      </c>
-      <c r="D159" s="1">
-        <v>3</v>
-      </c>
-      <c r="E159" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="F159" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="G159" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A160" s="1">
-        <v>2</v>
-      </c>
-      <c r="B160" s="1">
-        <v>15</v>
-      </c>
-      <c r="C160" s="1">
-        <v>30</v>
-      </c>
-      <c r="D160" s="1">
-        <v>3</v>
-      </c>
-      <c r="E160" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="F160" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="G160" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A161" s="1">
-        <v>2</v>
-      </c>
-      <c r="B161" s="1">
-        <v>16</v>
-      </c>
-      <c r="C161" s="1">
-        <v>31</v>
-      </c>
-      <c r="D161" s="1">
-        <v>3</v>
-      </c>
-      <c r="E161" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="F161" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="G161" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A162" s="1">
-        <v>2</v>
-      </c>
-      <c r="B162" s="1">
-        <v>17</v>
-      </c>
-      <c r="C162" s="1">
-        <v>32</v>
-      </c>
-      <c r="D162" s="1">
-        <v>3</v>
-      </c>
-      <c r="E162" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="F162" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="G162" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A163" s="1">
-        <v>2</v>
-      </c>
-      <c r="B163" s="1">
-        <v>18</v>
-      </c>
-      <c r="C163" s="1">
-        <v>33</v>
-      </c>
-      <c r="D163" s="1">
-        <v>3</v>
-      </c>
-      <c r="E163" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="F163" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="G163" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A164" s="1">
-        <v>2</v>
-      </c>
-      <c r="B164" s="1">
-        <v>19</v>
-      </c>
-      <c r="C164" s="1">
-        <v>34</v>
-      </c>
-      <c r="D164" s="1">
-        <v>3</v>
-      </c>
-      <c r="E164" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="F164" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="G164" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A165" s="1">
-        <v>2</v>
-      </c>
-      <c r="B165" s="1">
-        <v>20</v>
-      </c>
-      <c r="C165" s="1">
-        <v>35</v>
-      </c>
-      <c r="D165" s="1">
-        <v>3</v>
-      </c>
-      <c r="E165" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="F165" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="G165" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A166" s="1">
-        <v>2</v>
-      </c>
-      <c r="B166" s="1">
-        <v>21</v>
-      </c>
-      <c r="C166" s="1">
-        <v>36</v>
-      </c>
-      <c r="D166" s="1">
-        <v>3</v>
-      </c>
-      <c r="E166" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="F166" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="G166" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A167" s="1">
-        <v>2</v>
-      </c>
-      <c r="B167" s="1">
-        <v>22</v>
-      </c>
-      <c r="C167" s="1">
-        <v>37</v>
-      </c>
-      <c r="D167" s="1">
-        <v>3</v>
-      </c>
-      <c r="E167" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="F167" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="G167" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A168" s="1">
-        <v>2</v>
-      </c>
-      <c r="B168" s="1">
-        <v>23</v>
-      </c>
-      <c r="C168" s="1">
-        <v>38</v>
-      </c>
-      <c r="D168" s="1">
-        <v>3</v>
-      </c>
-      <c r="E168" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="F168" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="G168" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A169" s="1">
-        <v>2</v>
-      </c>
-      <c r="B169" s="1">
-        <v>24</v>
-      </c>
-      <c r="C169" s="1">
-        <v>39</v>
-      </c>
-      <c r="D169" s="1">
-        <v>3</v>
-      </c>
-      <c r="E169" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="F169" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="G169" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A170" s="1">
-        <v>2</v>
-      </c>
-      <c r="B170" s="1">
-        <v>25</v>
-      </c>
-      <c r="C170" s="1">
-        <v>84</v>
-      </c>
-      <c r="D170" s="1">
-        <v>6</v>
-      </c>
-      <c r="E170" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="F170" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="G170" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A171" s="1">
-        <v>2</v>
-      </c>
-      <c r="B171" s="1">
-        <v>26</v>
-      </c>
-      <c r="C171" s="1">
-        <v>85</v>
-      </c>
-      <c r="D171" s="1">
-        <v>6</v>
-      </c>
-      <c r="E171" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="F171" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="G171" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A172" s="1">
-        <v>2</v>
-      </c>
-      <c r="B172" s="1">
-        <v>27</v>
-      </c>
-      <c r="C172" s="1">
-        <v>86</v>
-      </c>
-      <c r="D172" s="1">
-        <v>6</v>
-      </c>
-      <c r="E172" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="F172" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="G172" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A173" s="1">
-        <v>2</v>
-      </c>
-      <c r="B173" s="1">
-        <v>28</v>
-      </c>
-      <c r="C173" s="1">
-        <v>87</v>
-      </c>
-      <c r="D173" s="1">
-        <v>6</v>
-      </c>
-      <c r="E173" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="F173" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="G173" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A174" s="1">
-        <v>2</v>
-      </c>
-      <c r="B174" s="1">
-        <v>29</v>
-      </c>
-      <c r="C174" s="1">
-        <v>88</v>
-      </c>
-      <c r="D174" s="1">
-        <v>6</v>
-      </c>
-      <c r="E174" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="F174" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="G174" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A175" s="1">
-        <v>2</v>
-      </c>
-      <c r="B175" s="1">
-        <v>30</v>
-      </c>
-      <c r="C175" s="1">
-        <v>89</v>
-      </c>
-      <c r="D175" s="1">
-        <v>6</v>
-      </c>
-      <c r="E175" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="F175" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="G175" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A176" s="1">
-        <v>2</v>
-      </c>
-      <c r="B176" s="1">
-        <v>31</v>
-      </c>
-      <c r="C176" s="1">
-        <v>90</v>
-      </c>
-      <c r="D176" s="1">
-        <v>6</v>
-      </c>
-      <c r="E176" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="F176" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="G176" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A177" s="1">
-        <v>2</v>
-      </c>
-      <c r="B177" s="1">
-        <v>32</v>
-      </c>
-      <c r="C177" s="1">
-        <v>91</v>
-      </c>
-      <c r="D177" s="1">
-        <v>6</v>
-      </c>
-      <c r="E177" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="F177" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="G177" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A178" s="1">
-        <v>2</v>
-      </c>
-      <c r="B178" s="1">
-        <v>33</v>
-      </c>
-      <c r="C178" s="1">
-        <v>92</v>
-      </c>
-      <c r="D178" s="1">
-        <v>6</v>
-      </c>
-      <c r="E178" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="F178" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="G178" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A179" s="1">
-        <v>2</v>
-      </c>
-      <c r="B179" s="1">
-        <v>34</v>
-      </c>
-      <c r="C179" s="1">
-        <v>93</v>
-      </c>
-      <c r="D179" s="1">
-        <v>6</v>
-      </c>
-      <c r="E179" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="F179" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="G179" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A180" s="1">
-        <v>2</v>
-      </c>
-      <c r="B180" s="1">
-        <v>35</v>
-      </c>
-      <c r="C180" s="1">
-        <v>94</v>
-      </c>
-      <c r="D180" s="1">
-        <v>6</v>
-      </c>
-      <c r="E180" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="F180" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="G180" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A181" s="1">
-        <v>2</v>
-      </c>
-      <c r="B181" s="1">
-        <v>36</v>
-      </c>
-      <c r="C181" s="1">
-        <v>95</v>
-      </c>
-      <c r="D181" s="1">
-        <v>6</v>
-      </c>
-      <c r="E181" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="F181" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="G181" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A182" s="1">
-        <v>2</v>
-      </c>
-      <c r="B182" s="1">
-        <v>37</v>
-      </c>
-      <c r="C182" s="1">
-        <v>96</v>
-      </c>
-      <c r="D182" s="1">
-        <v>6</v>
-      </c>
-      <c r="E182" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="F182" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="G182" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A183" s="1">
-        <v>2</v>
-      </c>
-      <c r="B183" s="1">
-        <v>38</v>
-      </c>
-      <c r="C183" s="1">
-        <v>97</v>
-      </c>
-      <c r="D183" s="1">
-        <v>6</v>
-      </c>
-      <c r="E183" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="F183" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="G183" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A184" s="1">
-        <v>2</v>
-      </c>
-      <c r="B184" s="1">
-        <v>39</v>
-      </c>
-      <c r="C184" s="1">
-        <v>98</v>
-      </c>
-      <c r="D184" s="1">
-        <v>6</v>
-      </c>
-      <c r="E184" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="F184" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="G184" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A185" s="1">
-        <v>6</v>
-      </c>
-      <c r="B185" s="1">
-        <v>1</v>
-      </c>
-      <c r="C185" s="1">
-        <v>145</v>
-      </c>
-      <c r="D185" s="1">
-        <v>10</v>
-      </c>
-      <c r="E185" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="F185" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="G185" s="1" t="s">
         <v>199</v>
       </c>
     </row>
@@ -17085,8 +16234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="C147" sqref="C147:C148"/>
+    <sheetView topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46:A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
creando el usuario 1 y 2
</commit_message>
<xml_diff>
--- a/provisional/inserts.xlsx
+++ b/provisional/inserts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="20640" windowHeight="10035" firstSheet="1" activeTab="8"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="20640" windowHeight="10035" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="inserts iniciales" sheetId="3" r:id="rId1"/>
@@ -1005,7 +1005,7 @@
     <t>Facturacion.frmFacturacion</t>
   </si>
   <si>
-    <t>Seguridad.frmAsignacionDeUsuariosAEmpresa</t>
+    <t>Seguridad.frmAsignarUsuariosAEmpresa</t>
   </si>
 </sst>
 </file>
@@ -17422,8 +17422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G157"/>
   <sheetViews>
-    <sheetView topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35462,7 +35462,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G242"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
+    <sheetView topLeftCell="A130" workbookViewId="0">
       <selection activeCell="G149" sqref="G149"/>
     </sheetView>
   </sheetViews>

</xml_diff>